<commit_message>
Data exploration for each features and data type in excel file.
</commit_message>
<xml_diff>
--- a/Data/Leads Data Dictionary.xlsx
+++ b/Data/Leads Data Dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\upgrad\Lead_scoring_proj\LeadScoring_gd\LeadScoring_ug\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E26ACB1B-4ACE-4F1E-BDA9-222EBE7FEC5F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{285DAB40-EE42-49A3-857C-DCD8F7C3B721}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7485" xr2:uid="{EB0EA90F-5D02-4555-A556-590372CD380C}"/>
+    <workbookView xWindow="19090" yWindow="-1920" windowWidth="38620" windowHeight="21100" xr2:uid="{EB0EA90F-5D02-4555-A556-590372CD380C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="91">
   <si>
     <t>Last Notable Activity</t>
   </si>
@@ -235,6 +235,75 @@
   </si>
   <si>
     <t>The target variable. Indicates whether a lead has been successfully converted or not.</t>
+  </si>
+  <si>
+    <t>NR</t>
+  </si>
+  <si>
+    <t>UID</t>
+  </si>
+  <si>
+    <t>Categorical</t>
+  </si>
+  <si>
+    <t>Binary</t>
+  </si>
+  <si>
+    <t>Numerical</t>
+  </si>
+  <si>
+    <t>Since Select is too high we need to assign 00 for this Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Unemployed 00</t>
+  </si>
+  <si>
+    <t>Can't be used as 99% in "Better Career prospects"</t>
+  </si>
+  <si>
+    <t>"Yes", "No" need to convert</t>
+  </si>
+  <si>
+    <t>Only "No" present</t>
+  </si>
+  <si>
+    <t>"Yes", "No" need to convert, No - 9238</t>
+  </si>
+  <si>
+    <t>"Yes", "No" need to convert, No - 9239</t>
+  </si>
+  <si>
+    <t>"Yes", "No" need to convert, No - 9236</t>
+  </si>
+  <si>
+    <t>"Yes", "No" need to convert, No - 9233</t>
+  </si>
+  <si>
+    <t>All "No" No need</t>
+  </si>
+  <si>
+    <t>Need Chi-square test</t>
+  </si>
+  <si>
+    <t>4 Categories, need One hot encoding</t>
+  </si>
+  <si>
+    <t>Many categories, need to bucket some rare categories together</t>
+  </si>
+  <si>
+    <t>"Yes", "No" No - 9238</t>
+  </si>
+  <si>
+    <t>"Yes", "No" No - 8506</t>
+  </si>
+  <si>
+    <t>0,1</t>
+  </si>
+  <si>
+    <t>Try Numerical or later bucket it</t>
+  </si>
+  <si>
+    <t>Need Boxplot to see importance</t>
   </si>
 </sst>
 </file>
@@ -336,7 +405,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -364,6 +433,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -679,10 +751,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65B9257A-60F9-4716-BB64-9F7B0F8B9298}">
-  <dimension ref="A3:C40"/>
+  <dimension ref="A3:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,9 +762,10 @@
     <col min="1" max="1" width="10.85546875" style="2" customWidth="1"/>
     <col min="2" max="2" width="16.85546875" style="2" customWidth="1"/>
     <col min="3" max="3" width="64.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="40.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>65</v>
       </c>
@@ -700,221 +773,368 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>31</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="6" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>29</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="7" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="8" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="9" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="10" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>71</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>71</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="12" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>72</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>24</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="13" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="14" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="16" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="17" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="18" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>70</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="19" spans="2:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>70</v>
+      </c>
+      <c r="E18" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
         <v>47</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="20" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>70</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>71</v>
+      </c>
+      <c r="E20" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C21" s="8"/>
-    </row>
-    <row r="22" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>71</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C22" s="8"/>
-    </row>
-    <row r="23" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>71</v>
+      </c>
+      <c r="E22" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
         <v>63</v>
       </c>
       <c r="C23" s="8"/>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>71</v>
+      </c>
+      <c r="E23" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C24" s="8"/>
-    </row>
-    <row r="25" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>71</v>
+      </c>
+      <c r="E24" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C25" s="9"/>
-    </row>
-    <row r="26" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>71</v>
+      </c>
+      <c r="E25" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="27" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>71</v>
+      </c>
+      <c r="E26" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>71</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="29" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>70</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="30" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>70</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="31" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>71</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>71</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
counting along with NA values
</commit_message>
<xml_diff>
--- a/Data/Leads Data Dictionary.xlsx
+++ b/Data/Leads Data Dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\upgrad\Lead_scoring_proj\LeadScoring_gd\LeadScoring_ug\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05F7BCDA-A338-4840-9BA1-00F1557A2A34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85C83857-D412-4B20-BA9B-532685CA6474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-1920" windowWidth="38620" windowHeight="21100" xr2:uid="{EB0EA90F-5D02-4555-A556-590372CD380C}"/>
   </bookViews>
@@ -405,7 +405,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -433,9 +433,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -753,8 +750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65B9257A-60F9-4716-BB64-9F7B0F8B9298}">
   <dimension ref="A3:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -805,7 +802,7 @@
       <c r="D6" t="s">
         <v>70</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="2" t="s">
         <v>84</v>
       </c>
     </row>
@@ -819,7 +816,7 @@
       <c r="D7" t="s">
         <v>70</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="2" t="s">
         <v>85</v>
       </c>
     </row>
@@ -833,7 +830,7 @@
       <c r="D8" t="s">
         <v>71</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="2" t="s">
         <v>87</v>
       </c>
     </row>
@@ -847,7 +844,7 @@
       <c r="D9" t="s">
         <v>71</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="2" t="s">
         <v>86</v>
       </c>
     </row>
@@ -861,7 +858,7 @@
       <c r="D10" t="s">
         <v>71</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="2" t="s">
         <v>88</v>
       </c>
     </row>
@@ -875,7 +872,7 @@
       <c r="D11" t="s">
         <v>72</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="2" t="s">
         <v>89</v>
       </c>
     </row>
@@ -944,7 +941,7 @@
       <c r="D17" t="s">
         <v>70</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="2" t="s">
         <v>73</v>
       </c>
     </row>
@@ -972,7 +969,7 @@
       <c r="D19" t="s">
         <v>70</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E19" s="2" t="s">
         <v>75</v>
       </c>
     </row>
@@ -998,7 +995,7 @@
       <c r="D21" t="s">
         <v>71</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E21" s="2" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1074,7 +1071,7 @@
       <c r="D27" t="s">
         <v>71</v>
       </c>
-      <c r="E27" s="10" t="s">
+      <c r="E27" s="2" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1088,7 +1085,7 @@
       <c r="D28" t="s">
         <v>70</v>
       </c>
-      <c r="E28" s="10" t="s">
+      <c r="E28" s="2" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1102,7 +1099,7 @@
       <c r="D29" t="s">
         <v>70</v>
       </c>
-      <c r="E29" s="10" t="s">
+      <c r="E29" s="2" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1116,7 +1113,7 @@
       <c r="D30" t="s">
         <v>71</v>
       </c>
-      <c r="E30" s="10" t="s">
+      <c r="E30" s="2" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1130,7 +1127,7 @@
       <c r="D31" t="s">
         <v>71</v>
       </c>
-      <c r="E31" s="10" t="s">
+      <c r="E31" s="2" t="s">
         <v>82</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Categorical variable eda using chi-square test and Bixplot and value counts
</commit_message>
<xml_diff>
--- a/Data/Leads Data Dictionary.xlsx
+++ b/Data/Leads Data Dictionary.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\upgrad\Lead_scoring_proj\LeadScoring_gd\LeadScoring_ug\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85C83857-D412-4B20-BA9B-532685CA6474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2094A20-0B95-480C-A7D4-E0B53024778C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-1920" windowWidth="38620" windowHeight="21100" xr2:uid="{EB0EA90F-5D02-4555-A556-590372CD380C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$3:$E$40</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="95">
   <si>
     <t>Last Notable Activity</t>
   </si>
@@ -304,6 +307,18 @@
   </si>
   <si>
     <t>Need Boxplot to see importance</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Catgeorical</t>
+  </si>
+  <si>
+    <t>All No, No need</t>
+  </si>
+  <si>
+    <t>Needed</t>
   </si>
 </sst>
 </file>
@@ -405,7 +420,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -433,6 +448,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -748,10 +766,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65B9257A-60F9-4716-BB64-9F7B0F8B9298}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A3:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -769,8 +788,11 @@
       <c r="C3" s="6" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>31</v>
       </c>
@@ -781,7 +803,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>30</v>
       </c>
@@ -862,7 +884,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>25</v>
       </c>
@@ -876,7 +898,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>24</v>
       </c>
@@ -887,7 +909,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
         <v>23</v>
       </c>
@@ -1138,66 +1160,111 @@
       <c r="C32" s="3" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
         <v>64</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="34" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="35" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B35" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C35" s="8"/>
-    </row>
-    <row r="36" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B36" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C36" s="8"/>
-    </row>
-    <row r="37" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B37" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C37" s="9"/>
-    </row>
-    <row r="38" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B38" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="39" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>92</v>
+      </c>
+      <c r="E38" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B39" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="40" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>70</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B40" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>62</v>
       </c>
+      <c r="D40" t="s">
+        <v>70</v>
+      </c>
+      <c r="E40" s="10" t="s">
+        <v>94</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A3:E40" xr:uid="{65B9257A-60F9-4716-BB64-9F7B0F8B9298}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="Binary"/>
+        <filter val="Categorical"/>
+        <filter val="Catgeorical"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="2">
     <mergeCell ref="C20:C25"/>
     <mergeCell ref="C34:C37"/>

</xml_diff>